<commit_message>
Replaced [employee] with updated version
</commit_message>
<xml_diff>
--- a/Cleaned_Employee_Data.xlsx
+++ b/Cleaned_Employee_Data.xlsx
@@ -9517,7 +9517,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>unkown</t>
+          <t>Not Provided</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -9709,7 +9709,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>unkown</t>
+          <t>Not Provided</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">

</xml_diff>